<commit_message>
Added advise on PROGn, INITn, DONE pins
</commit_message>
<xml_diff>
--- a/docs/misc/tinyCLUNX_baseboard_review_items.xlsx
+++ b/docs/misc/tinyCLUNX_baseboard_review_items.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\github\tinyclunx33_public\Docs\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ABB24FB-F727-4FE9-BD57-C257F1605315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B96F103-C42D-469E-9CE7-CAADC876DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18180" yWindow="8868" windowWidth="18408" windowHeight="15348" xr2:uid="{1CCB57F0-CF8C-4ADC-A4C1-F8C725608D0F}"/>
+    <workbookView xWindow="26772" yWindow="4968" windowWidth="15036" windowHeight="16476" activeTab="1" xr2:uid="{1CCB57F0-CF8C-4ADC-A4C1-F8C725608D0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Schematic" sheetId="2" r:id="rId1"/>
     <sheet name="Layout" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
-  <si>
-    <t>Check MIPI intra pair length matches</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Check MIPI clock to data inter-pair match</t>
   </si>
@@ -52,9 +48,6 @@
     <t>USB3 SS diff pair intra pair match</t>
   </si>
   <si>
-    <t>VBUS conencted to USB 5V</t>
-  </si>
-  <si>
     <t>Bank voltage allocation</t>
   </si>
   <si>
@@ -172,22 +165,31 @@
     <t>JTAG connections brought out ffor debug/programming</t>
   </si>
   <si>
-    <t>DONE pin should not be pulled low during FPGA boot up, this is an open drain.</t>
-  </si>
-  <si>
     <t>Add B1_RXD and G1_TXD for UART debug to at least test points</t>
   </si>
   <si>
     <t>Bank 2/3/4 used for MIPI signals shall be 1.2V</t>
   </si>
   <si>
-    <t>1.8V/3.3V sourced from SoM consumes no more than 1.8V</t>
-  </si>
-  <si>
     <t>Unused bank voltage pins on the Compute SoM (J1B:58, 60) are hooked up to 1.8V for compatibility with Connectivity module</t>
   </si>
   <si>
     <t>ESD protection on USB lines</t>
+  </si>
+  <si>
+    <t>INITn, PROGn, DONE pin should not be pulled low during FPGA boot up, this is an open drain.</t>
+  </si>
+  <si>
+    <t>1.8V/3.3V sourced from SoM consumes no more than 800mA</t>
+  </si>
+  <si>
+    <t>VBUS connected to USB 5V</t>
+  </si>
+  <si>
+    <t>Power enable must be high to turn on the SoM</t>
+  </si>
+  <si>
+    <t>Check MIPI intra pair length match</t>
   </si>
 </sst>
 </file>
@@ -568,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8948F76-05E6-40B5-A62D-242DFA8C4EA7}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,148 +585,153 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+      <c r="A6" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>46</v>
+      <c r="A24" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D67E7C8-0554-4C4F-BB91-DD4AAD3BB3A0}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -745,7 +754,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -753,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -761,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -769,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -777,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -785,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -793,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -801,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -809,7 +818,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -817,7 +826,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -825,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -833,7 +842,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,7 +850,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -849,7 +858,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -857,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -865,7 +874,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -873,7 +882,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -881,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -889,7 +898,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -897,7 +906,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -905,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -913,7 +922,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>